<commit_message>
Reporte Secundario Faena excel - Se quitan reportes pdf
</commit_message>
<xml_diff>
--- a/carga/REPORTE 1.1.xlsx
+++ b/carga/REPORTE 1.1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ORNELA\Documents\BARLOVENTO SRL\ANALISIS INFORMACIÓN GANADERA BASE DATOS\REPORTES1, 2, 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mamauuro\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABA5A68-91B6-4524-B91A-236E3EDC5BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Informe_Carpeta_Prueba1234 (1)" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="28">
   <si>
     <t>Informe de Carpeta</t>
   </si>
@@ -104,12 +103,15 @@
   </si>
   <si>
     <t>Desv. Est.</t>
+  </si>
+  <si>
+    <t>Hembra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -639,7 +641,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -669,6 +671,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1025,26 +1033,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1063,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1066,7 +1074,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1079,7 +1087,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1092,7 +1100,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1109,7 +1117,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -1126,7 +1134,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1152,7 +1160,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>45082</v>
       </c>
@@ -1176,7 +1184,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>45082</v>
       </c>
@@ -1200,7 +1208,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45082</v>
       </c>
@@ -1224,7 +1232,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>45082</v>
       </c>
@@ -1248,7 +1256,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>45082</v>
       </c>
@@ -1272,7 +1280,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>45082</v>
       </c>
@@ -1296,7 +1304,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>45082</v>
       </c>
@@ -1320,7 +1328,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>45082</v>
       </c>
@@ -1344,7 +1352,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>45082</v>
       </c>
@@ -1368,7 +1376,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>45082</v>
       </c>
@@ -1392,7 +1400,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>45082</v>
       </c>
@@ -1416,7 +1424,7 @@
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>45082</v>
       </c>
@@ -1440,7 +1448,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>45082</v>
       </c>
@@ -1464,7 +1472,7 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>45082</v>
       </c>
@@ -1488,7 +1496,7 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>45082</v>
       </c>
@@ -1512,7 +1520,7 @@
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>45082</v>
       </c>
@@ -1536,7 +1544,7 @@
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>45082</v>
       </c>
@@ -1560,7 +1568,7 @@
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>45082</v>
       </c>
@@ -1584,7 +1592,7 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>45082</v>
       </c>
@@ -1608,7 +1616,7 @@
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>45082</v>
       </c>
@@ -1632,7 +1640,7 @@
       </c>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>45082</v>
       </c>
@@ -1656,7 +1664,7 @@
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>45082</v>
       </c>
@@ -1680,7 +1688,7 @@
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>45082</v>
       </c>
@@ -1704,7 +1712,7 @@
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>45082</v>
       </c>
@@ -1728,49 +1736,433 @@
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B32" s="11">
+        <v>21496</v>
+      </c>
+      <c r="C32" s="11">
+        <v>13</v>
+      </c>
+      <c r="D32" s="11">
+        <v>329</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="11">
+        <v>0</v>
+      </c>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B33" s="11">
+        <v>21638</v>
+      </c>
+      <c r="C33" s="11">
+        <v>10</v>
+      </c>
+      <c r="D33" s="11">
+        <v>339</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="11">
+        <v>0</v>
+      </c>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B34" s="11">
+        <v>21753</v>
+      </c>
+      <c r="C34" s="11">
+        <v>10</v>
+      </c>
+      <c r="D34" s="11">
+        <v>361</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="11">
+        <v>0</v>
+      </c>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B35" s="11">
+        <v>32161</v>
+      </c>
+      <c r="C35" s="11">
+        <v>9</v>
+      </c>
+      <c r="D35" s="11">
+        <v>341</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="11">
+        <v>0</v>
+      </c>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B36" s="11">
+        <v>32450</v>
+      </c>
+      <c r="C36" s="11">
+        <v>8</v>
+      </c>
+      <c r="D36" s="11">
+        <v>335</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="11">
+        <v>0</v>
+      </c>
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B37" s="11">
+        <v>32634</v>
+      </c>
+      <c r="C37" s="11">
+        <v>5</v>
+      </c>
+      <c r="D37" s="11">
+        <v>359</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="11">
+        <v>0</v>
+      </c>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B38" s="11">
+        <v>32725</v>
+      </c>
+      <c r="C38" s="11">
+        <v>7</v>
+      </c>
+      <c r="D38" s="11">
+        <v>332</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="11">
+        <v>0</v>
+      </c>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B39" s="11">
+        <v>32807</v>
+      </c>
+      <c r="C39" s="11">
+        <v>7</v>
+      </c>
+      <c r="D39" s="11">
+        <v>342</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="11">
+        <v>0</v>
+      </c>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B40" s="11">
+        <v>33687</v>
+      </c>
+      <c r="C40" s="11">
+        <v>9</v>
+      </c>
+      <c r="D40" s="11">
+        <v>341</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="11">
+        <v>0</v>
+      </c>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B41" s="11">
+        <v>33687</v>
+      </c>
+      <c r="C41" s="11">
+        <v>16</v>
+      </c>
+      <c r="D41" s="11">
+        <v>341</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="11">
+        <v>0</v>
+      </c>
+      <c r="H41" s="11"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B42" s="11">
+        <v>33689</v>
+      </c>
+      <c r="C42" s="11">
+        <v>4</v>
+      </c>
+      <c r="D42" s="11">
+        <v>340</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="11">
+        <v>0</v>
+      </c>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B43" s="11">
+        <v>34123</v>
+      </c>
+      <c r="C43" s="11">
+        <v>12</v>
+      </c>
+      <c r="D43" s="11">
+        <v>356</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="11">
+        <v>0</v>
+      </c>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B44" s="11">
+        <v>34404</v>
+      </c>
+      <c r="C44" s="11">
+        <v>10</v>
+      </c>
+      <c r="D44" s="11">
+        <v>365</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="11">
+        <v>0</v>
+      </c>
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B45" s="11">
+        <v>34468</v>
+      </c>
+      <c r="C45" s="11">
+        <v>11</v>
+      </c>
+      <c r="D45" s="11">
+        <v>352</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="11">
+        <v>0</v>
+      </c>
+      <c r="H45" s="11"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B46" s="11">
+        <v>50483</v>
+      </c>
+      <c r="C46" s="11">
+        <v>8</v>
+      </c>
+      <c r="D46" s="11">
+        <v>327</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="11">
+        <v>0</v>
+      </c>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="12">
+        <v>45082</v>
+      </c>
+      <c r="B47" s="11">
+        <v>50490</v>
+      </c>
+      <c r="C47" s="11">
+        <v>13</v>
+      </c>
+      <c r="D47" s="11">
+        <v>343</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" s="11">
+        <v>0</v>
+      </c>
+      <c r="H47" s="11"/>
+    </row>
+    <row r="48" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
+      <c r="F48" s="5"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
         <v>10610.8</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B49" s="1">
         <v>442.11666666667003</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C49" s="1">
         <v>377.6</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D49" s="1">
         <v>495.2</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E49" s="1">
         <v>34.770000000000003</v>
       </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="6"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:H7" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A7:H7"/>
   <mergeCells count="8">
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:G3"/>

</xml_diff>

<commit_message>
Validar Rfid repetido en planillas
</commit_message>
<xml_diff>
--- a/carga/REPORTE 1.1.xlsx
+++ b/carga/REPORTE 1.1.xlsx
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Informe_Carpeta_Prueba1234 (1)'!$A$7:$H$7</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="28">
   <si>
     <t>Informe de Carpeta</t>
   </si>
@@ -655,6 +655,12 @@
     <xf numFmtId="14" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -671,12 +677,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1034,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,26 +1053,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1081,11 +1081,11 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1094,11 +1094,11 @@
       <c r="B4" s="4">
         <v>45082</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1113,9 +1113,9 @@
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -1130,9 +1130,9 @@
       <c r="D6" s="1">
         <v>500</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1737,432 +1737,408 @@
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B32" s="11">
+      <c r="A32" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B32" s="5">
         <v>21496</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="5">
         <v>13</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="5">
         <v>329</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="11">
-        <v>0</v>
-      </c>
-      <c r="H32" s="11"/>
+      <c r="G32" s="5">
+        <v>0</v>
+      </c>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B33" s="11">
+      <c r="A33" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B33" s="5">
         <v>21638</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="5">
         <v>10</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="5">
         <v>339</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G33" s="11">
-        <v>0</v>
-      </c>
-      <c r="H33" s="11"/>
+      <c r="G33" s="5">
+        <v>0</v>
+      </c>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B34" s="11">
+      <c r="A34" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B34" s="5">
         <v>21753</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="5">
         <v>10</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="5">
         <v>361</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="11">
-        <v>0</v>
-      </c>
-      <c r="H34" s="11"/>
+      <c r="G34" s="5">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B35" s="11">
+      <c r="A35" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B35" s="5">
         <v>32161</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="5">
         <v>9</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="5">
         <v>341</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="11">
-        <v>0</v>
-      </c>
-      <c r="H35" s="11"/>
+      <c r="G35" s="5">
+        <v>0</v>
+      </c>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B36" s="11">
+      <c r="A36" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B36" s="5">
         <v>32450</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="5">
         <v>8</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="5">
         <v>335</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="11">
-        <v>0</v>
-      </c>
-      <c r="H36" s="11"/>
+      <c r="G36" s="5">
+        <v>0</v>
+      </c>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B37" s="11">
+      <c r="A37" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B37" s="5">
         <v>32634</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="5">
         <v>5</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="5">
         <v>359</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="11">
-        <v>0</v>
-      </c>
-      <c r="H37" s="11"/>
+      <c r="G37" s="5">
+        <v>0</v>
+      </c>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B38" s="11">
+      <c r="A38" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B38" s="5">
         <v>32725</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="5">
         <v>7</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="5">
         <v>332</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="11">
-        <v>0</v>
-      </c>
-      <c r="H38" s="11"/>
+      <c r="G38" s="5">
+        <v>0</v>
+      </c>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B39" s="11">
+      <c r="A39" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B39" s="5">
         <v>32807</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="5">
         <v>7</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="5">
         <v>342</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="11">
-        <v>0</v>
-      </c>
-      <c r="H39" s="11"/>
+      <c r="G39" s="5">
+        <v>0</v>
+      </c>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B40" s="11">
+      <c r="A40" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B40" s="5">
         <v>33687</v>
       </c>
-      <c r="C40" s="11">
-        <v>9</v>
-      </c>
-      <c r="D40" s="11">
+      <c r="C40" s="5">
+        <v>16</v>
+      </c>
+      <c r="D40" s="5">
         <v>341</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0</v>
+      </c>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B41" s="5">
+        <v>33689</v>
+      </c>
+      <c r="C41" s="5">
+        <v>4</v>
+      </c>
+      <c r="D41" s="5">
+        <v>340</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B42" s="5">
+        <v>34123</v>
+      </c>
+      <c r="C42" s="5">
+        <v>12</v>
+      </c>
+      <c r="D42" s="5">
+        <v>356</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B43" s="5">
+        <v>34404</v>
+      </c>
+      <c r="C43" s="5">
+        <v>10</v>
+      </c>
+      <c r="D43" s="5">
+        <v>365</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G40" s="11">
-        <v>0</v>
-      </c>
-      <c r="H40" s="11"/>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B41" s="11">
-        <v>33687</v>
-      </c>
-      <c r="C41" s="11">
-        <v>16</v>
-      </c>
-      <c r="D41" s="11">
-        <v>341</v>
-      </c>
-      <c r="E41" s="11" t="s">
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B44" s="5">
+        <v>34468</v>
+      </c>
+      <c r="C44" s="5">
+        <v>11</v>
+      </c>
+      <c r="D44" s="5">
+        <v>352</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B45" s="5">
+        <v>50483</v>
+      </c>
+      <c r="C45" s="5">
+        <v>8</v>
+      </c>
+      <c r="D45" s="5">
+        <v>327</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0</v>
+      </c>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>45082</v>
+      </c>
+      <c r="B46" s="5">
+        <v>50490</v>
+      </c>
+      <c r="C46" s="5">
+        <v>13</v>
+      </c>
+      <c r="D46" s="5">
+        <v>343</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G41" s="11">
-        <v>0</v>
-      </c>
-      <c r="H41" s="11"/>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B42" s="11">
-        <v>33689</v>
-      </c>
-      <c r="C42" s="11">
-        <v>4</v>
-      </c>
-      <c r="D42" s="11">
-        <v>340</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="11">
-        <v>0</v>
-      </c>
-      <c r="H42" s="11"/>
-    </row>
-    <row r="43" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B43" s="11">
-        <v>34123</v>
-      </c>
-      <c r="C43" s="11">
-        <v>12</v>
-      </c>
-      <c r="D43" s="11">
-        <v>356</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G43" s="11">
-        <v>0</v>
-      </c>
-      <c r="H43" s="11"/>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B44" s="11">
-        <v>34404</v>
-      </c>
-      <c r="C44" s="11">
-        <v>10</v>
-      </c>
-      <c r="D44" s="11">
-        <v>365</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="11">
-        <v>0</v>
-      </c>
-      <c r="H44" s="11"/>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B45" s="11">
-        <v>34468</v>
-      </c>
-      <c r="C45" s="11">
-        <v>11</v>
-      </c>
-      <c r="D45" s="11">
-        <v>352</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="11">
-        <v>0</v>
-      </c>
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B46" s="11">
-        <v>50483</v>
-      </c>
-      <c r="C46" s="11">
+      <c r="G46" s="5">
+        <v>0</v>
+      </c>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="11">
-        <v>327</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G46" s="11">
-        <v>0</v>
-      </c>
-      <c r="H46" s="11"/>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12">
-        <v>45082</v>
-      </c>
-      <c r="B47" s="11">
-        <v>50490</v>
-      </c>
-      <c r="C47" s="11">
-        <v>13</v>
-      </c>
-      <c r="D47" s="11">
-        <v>343</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G47" s="11">
-        <v>0</v>
-      </c>
-      <c r="H47" s="11"/>
-    </row>
-    <row r="48" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="5"/>
-      <c r="G48" s="6"/>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
+      <c r="F47" s="7"/>
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
         <v>10610.8</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B48" s="1">
         <v>442.11666666667003</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C48" s="1">
         <v>377.6</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D48" s="1">
         <v>495.2</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E48" s="1">
         <v>34.770000000000003</v>
       </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="6"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A7:H7"/>
   <mergeCells count="8">
+    <mergeCell ref="F47:G47"/>
     <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:G3"/>

</xml_diff>